<commit_message>
Add more square questions
</commit_message>
<xml_diff>
--- a/company/lyft/lyft-freq.xlsx
+++ b/company/lyft/lyft-freq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bozhou/Dropbox/interview/company/lyft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A3E4C6-B245-E14B-A244-9845D6A307DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E750D90E-7DCD-124F-8E6D-89DC2A2E9850}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47560" yWindow="2820" windowWidth="22420" windowHeight="18100" xr2:uid="{E083BCA1-116D-FE4F-8F8A-D54DCBD9886C}"/>
+    <workbookView xWindow="2860" yWindow="460" windowWidth="20620" windowHeight="13320" xr2:uid="{E083BCA1-116D-FE4F-8F8A-D54DCBD9886C}"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithm" sheetId="1" r:id="rId1"/>
@@ -627,7 +627,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>